<commit_message>
finaliza o dicionario de dados
</commit_message>
<xml_diff>
--- a/banco/documentacao/Dicionário de dados.xlsx
+++ b/banco/documentacao/Dicionário de dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago\Desktop\PetAgenda\banco\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031778B2-3CE6-4920-AD36-3247D44864B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC967D6-5A81-451E-ADFC-9DB670174EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="212">
   <si>
     <t>cliente</t>
   </si>
@@ -346,9 +346,6 @@
     <t>Tempo, em minutos, que levou para o serviço ser concluído.</t>
   </si>
   <si>
-    <t>servico_disponível</t>
-  </si>
-  <si>
     <t>Chave primária de identificação do cliente.</t>
   </si>
   <si>
@@ -521,6 +518,144 @@
   </si>
   <si>
     <t>Chave primária da área de atuação.</t>
+  </si>
+  <si>
+    <t>"descricao"</t>
+  </si>
+  <si>
+    <t>Chave primária do serviço disponível.</t>
+  </si>
+  <si>
+    <t>Nome descritivo do serviço disponível.</t>
+  </si>
+  <si>
+    <t>Tipo deste serviço. Chave estrangeira da tabela "tipo_servico".</t>
+  </si>
+  <si>
+    <t>Duração do serviço em minutos.</t>
+  </si>
+  <si>
+    <t>Preço do serviço.</t>
+  </si>
+  <si>
+    <t>Descrição do serviço.</t>
+  </si>
+  <si>
+    <t>1970-10-12 18:59:12</t>
+  </si>
+  <si>
+    <t>Chave primária do incidente.</t>
+  </si>
+  <si>
+    <t>Data e hora de quando o incidente ocorreu.</t>
+  </si>
+  <si>
+    <t>Condição de se o incidente é uma emergência. TRUE representa uma emergência, enquanto que FALSE não representa uma emergência.</t>
+  </si>
+  <si>
+    <t>Pet envolvido no incidente. Chave estrangeira da tabela "pet".</t>
+  </si>
+  <si>
+    <t>Serviço em que o incidente ocorreu. Chave estrangeira da tabela "servico_disponivel".</t>
+  </si>
+  <si>
+    <t>Descrição do incidente.</t>
+  </si>
+  <si>
+    <t>agendamento</t>
+  </si>
+  <si>
+    <t>Serviço agendado. Chave estrangeira da tabela "servico_disponivel".</t>
+  </si>
+  <si>
+    <t>Tipo do serviço agendado. Chave estrangeira da tabela "tipo_servico".</t>
+  </si>
+  <si>
+    <t>Data e hora agendadas.</t>
+  </si>
+  <si>
+    <t>"rua tal, numero 1, cidade..."</t>
+  </si>
+  <si>
+    <t>Pet que receberá o serviço agendado. Chave estrangeira da tabela "pet".</t>
+  </si>
+  <si>
+    <t>"observação"</t>
+  </si>
+  <si>
+    <t>"fulado"</t>
+  </si>
+  <si>
+    <t>"beltrano"</t>
+  </si>
+  <si>
+    <t>"clinica dos cuidados"</t>
+  </si>
+  <si>
+    <t>Funcionário responsável pelo serviço agendado. Chave estrangeira da tabela "usuario".</t>
+  </si>
+  <si>
+    <t>Observação do agendamento.</t>
+  </si>
+  <si>
+    <t>Pacote em que este agendamento está inserido. Deverá ser vazio se não estiver relacionado a nenhum pacote de agendamento.</t>
+  </si>
+  <si>
+    <t>Quantiadade de passeios que o Pet deverá receber, caso seja um serviço de Atendimento Doméstico.</t>
+  </si>
+  <si>
+    <t>Local onde o serviço do tipo Cuidado Especial ocorrerá.</t>
+  </si>
+  <si>
+    <t>Chave primária do pacote de agendamento.</t>
+  </si>
+  <si>
+    <t>"remédio"</t>
+  </si>
+  <si>
+    <t>"instruções"</t>
+  </si>
+  <si>
+    <t>Chave estrangeira da tabela "agendamento".</t>
+  </si>
+  <si>
+    <t>Remédio que deverá ser administrado ao Pet.</t>
+  </si>
+  <si>
+    <t>Horário em que o remédio deverá ser administrado.</t>
+  </si>
+  <si>
+    <t>Instruções adicionais de administração do remédio.</t>
+  </si>
+  <si>
+    <t>Horário em que o Pet deverá ser alimentado.</t>
+  </si>
+  <si>
+    <t>"nome do arquivo"</t>
+  </si>
+  <si>
+    <t>"C:\User\Public\receita.pdf"</t>
+  </si>
+  <si>
+    <t>Nome do arquivo em anexo.</t>
+  </si>
+  <si>
+    <t>Caminho do arquivo em anexo.</t>
+  </si>
+  <si>
+    <t>Descrição do que ocorreu durante o serviço.</t>
+  </si>
+  <si>
+    <t>Horário em que o serviço foi finalizado.</t>
+  </si>
+  <si>
+    <t>Observação do serviço ocorrido.</t>
+  </si>
+  <si>
+    <t>Comportamento do Pet durante a execução do serviço.</t>
+  </si>
+  <si>
+    <t>Chave estrangeira do incidente na tabela "incidente" caso haja um incidente relacionado a este serviço realizado.</t>
   </si>
 </sst>
 </file>
@@ -723,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -746,18 +881,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,13 +893,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1050,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G134" sqref="G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1064,23 +1205,23 @@
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" style="11" customWidth="1"/>
     <col min="8" max="8" width="25.140625" customWidth="1"/>
     <col min="9" max="12" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1096,8 +1237,8 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>111</v>
+      <c r="F2" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>6</v>
@@ -1119,11 +1260,11 @@
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>109</v>
+      <c r="G3" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1142,11 +1283,11 @@
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>117</v>
+      <c r="G4" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1166,8 +1307,8 @@
         <v>11</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="11" t="s">
-        <v>110</v>
+      <c r="G5" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,11 +1325,11 @@
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1207,11 +1348,11 @@
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1228,11 +1369,11 @@
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>118</v>
+      <c r="G8" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,11 +1390,11 @@
       <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>119</v>
+      <c r="F9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1270,24 +1411,24 @@
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>120</v>
+      <c r="F10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -1305,8 +1446,8 @@
       <c r="E13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>111</v>
+      <c r="F13" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>6</v>
@@ -1328,11 +1469,11 @@
       <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>121</v>
+      <c r="G14" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1351,11 +1492,11 @@
       <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>122</v>
+      <c r="G15" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1374,11 +1515,11 @@
       <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>130</v>
+      <c r="F16" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1395,11 +1536,11 @@
       <c r="E17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>131</v>
+      <c r="F17" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1418,11 +1559,11 @@
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>132</v>
+      <c r="F18" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1441,11 +1582,11 @@
       <c r="E19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>138</v>
+      <c r="F19" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1462,11 +1603,11 @@
       <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>133</v>
+      <c r="F20" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1483,11 +1624,11 @@
       <c r="E21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>134</v>
+      <c r="F21" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1501,14 +1642,14 @@
         <v>41</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>135</v>
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1522,14 +1663,14 @@
         <v>255</v>
       </c>
       <c r="D23" s="7"/>
-      <c r="E23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>136</v>
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1547,21 +1688,21 @@
         <v>11</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="11" t="s">
-        <v>137</v>
+      <c r="G24" s="8" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="10"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
@@ -1579,8 +1720,8 @@
       <c r="E27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>111</v>
+      <c r="F27" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>6</v>
@@ -1602,11 +1743,11 @@
       <c r="E28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>142</v>
+      <c r="G28" s="8" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1625,11 +1766,11 @@
       <c r="E29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>143</v>
+      <c r="F29" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1648,11 +1789,11 @@
       <c r="E30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>141</v>
+      <c r="G30" s="8" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1669,11 +1810,11 @@
       <c r="E31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1692,11 +1833,11 @@
       <c r="E32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>140</v>
+      <c r="F32" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1713,11 +1854,11 @@
       <c r="E33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>144</v>
+      <c r="F33" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1736,11 +1877,11 @@
       <c r="E34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>145</v>
+      <c r="F34" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1759,11 +1900,11 @@
       <c r="E35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>146</v>
+      <c r="F35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1780,25 +1921,25 @@
       <c r="E36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>147</v>
+      <c r="F36" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="10"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
@@ -1816,8 +1957,8 @@
       <c r="E40" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="18" t="s">
-        <v>111</v>
+      <c r="F40" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>6</v>
@@ -1839,11 +1980,11 @@
       <c r="E41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G41" s="11" t="s">
-        <v>153</v>
+      <c r="G41" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1862,11 +2003,11 @@
       <c r="E42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>154</v>
+      <c r="F42" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1885,11 +2026,11 @@
       <c r="E43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>155</v>
+      <c r="F43" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1908,11 +2049,11 @@
       <c r="E44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>156</v>
+      <c r="F44" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1931,11 +2072,11 @@
       <c r="E45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>157</v>
+      <c r="F45" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1952,29 +2093,29 @@
       <c r="E46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>158</v>
+      <c r="F46" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F47" s="20"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F48" s="20"/>
+      <c r="F48" s="13"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="10"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="16"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
@@ -1992,8 +2133,8 @@
       <c r="E50" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="18" t="s">
-        <v>111</v>
+      <c r="F50" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>6</v>
@@ -2015,11 +2156,11 @@
       <c r="E51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>159</v>
+      <c r="G51" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2038,24 +2179,24 @@
       <c r="E52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>160</v>
+      <c r="F52" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="10"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="16"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
@@ -2073,8 +2214,8 @@
       <c r="E55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="18" t="s">
-        <v>111</v>
+      <c r="F55" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>6</v>
@@ -2096,11 +2237,11 @@
       <c r="E56" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G56" s="11" t="s">
-        <v>162</v>
+      <c r="G56" s="8" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2119,24 +2260,24 @@
       <c r="E57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F57" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>163</v>
+      <c r="F57" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="10"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="16"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
@@ -2154,8 +2295,8 @@
       <c r="E60" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="18" t="s">
-        <v>111</v>
+      <c r="F60" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>6</v>
@@ -2177,11 +2318,11 @@
       <c r="E61" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G61" s="11" t="s">
-        <v>166</v>
+      <c r="G61" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2200,11 +2341,11 @@
       <c r="E62" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>164</v>
+      <c r="F62" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2223,26 +2364,26 @@
       <c r="E63" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F63" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>165</v>
+      <c r="F63" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="10"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="16"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
@@ -2260,8 +2401,8 @@
       <c r="E68" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="18" t="s">
-        <v>111</v>
+      <c r="F68" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>6</v>
@@ -2283,10 +2424,12 @@
       <c r="E69" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G69" s="4"/>
+      <c r="G69" s="4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
@@ -2301,11 +2444,17 @@
       <c r="D70" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E70" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>62</v>
       </c>
@@ -2318,11 +2467,15 @@
       <c r="D71" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="11" t="s">
+      <c r="E71" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G71" s="4"/>
+      <c r="G71" s="4" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
@@ -2337,11 +2490,15 @@
       <c r="D72" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="11" t="s">
+      <c r="E72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G72" s="4"/>
+      <c r="G72" s="8" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
@@ -2356,9 +2513,15 @@
       <c r="D73" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
@@ -2371,946 +2534,1087 @@
         <v>200</v>
       </c>
       <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="E74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="16"/>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="10"/>
+      <c r="A79" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B86" s="15"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="16"/>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D87" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E87" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F80" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G80" s="6" t="s">
+      <c r="F87" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G87" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+    <row r="88" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C88" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D88" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E81" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="11" t="s">
+      <c r="E88" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G81" s="4"/>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C82" s="11" t="s">
+      <c r="G88" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B84" s="11" t="s">
+      <c r="G89" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C90" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D90" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="11" t="s">
+      <c r="E90" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E85" s="4"/>
-      <c r="F85" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="10"/>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F89" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G90" s="4"/>
+      <c r="G90" s="8" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B91" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C92" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D92" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E91" s="4"/>
-      <c r="F91" s="11" t="s">
+      <c r="E92" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G91" s="4"/>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B92" s="11" t="s">
+      <c r="G92" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C94" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="D94" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="11" t="s">
+      <c r="E94" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G92" s="4"/>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="11" t="s">
+      <c r="G94" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D95" s="8"/>
+      <c r="E95" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4">
+        <v>0</v>
+      </c>
+      <c r="F99" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G99" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" s="15"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="16"/>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" s="15"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="16"/>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G108" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="22">
+        <v>0.7911111111111111</v>
+      </c>
+      <c r="G110" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D111" s="10"/>
+      <c r="E111" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B113" s="15"/>
+      <c r="C113" s="15"/>
+      <c r="D113" s="15"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="16"/>
+    </row>
+    <row r="114" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F114" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" s="22">
+        <v>0.7911111111111111</v>
+      </c>
+      <c r="G116" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B119" s="15"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="16"/>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F120" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G121" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="G122" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G123" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B125" s="15"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="16"/>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F126" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G126" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G127" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D128" s="8"/>
+      <c r="E128" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G128" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C129" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="D129" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B94" s="11" t="s">
+      <c r="E129" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G129" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C130" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D94" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E94" s="4"/>
-      <c r="F94" s="11" t="s">
+      <c r="D130" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="1:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95" s="4" t="s">
+      <c r="G130" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B131" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C131" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D95" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B96" s="11" t="s">
+      <c r="D131" s="8"/>
+      <c r="E131" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G131" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D132" s="8"/>
+      <c r="E132" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G132" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C133" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D96" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E96" s="4"/>
-      <c r="F96" s="11" t="s">
+      <c r="D133" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G96" s="4"/>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D97" s="11"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G98" s="4"/>
-    </row>
-    <row r="99" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4">
-        <v>0</v>
-      </c>
-      <c r="F101" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G101" s="4"/>
-    </row>
-    <row r="102" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D102" s="4"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-    </row>
-    <row r="103" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B104" s="9"/>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="10"/>
-    </row>
-    <row r="105" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F105" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E106" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-    </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B108" s="9"/>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="10"/>
-    </row>
-    <row r="109" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F109" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E110" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F110" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G110" s="4"/>
-    </row>
-    <row r="111" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C111" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-    </row>
-    <row r="112" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-    </row>
-    <row r="113" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D113" s="14"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-    </row>
-    <row r="114" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-    </row>
-    <row r="115" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B116" s="9"/>
-      <c r="C116" s="9"/>
-      <c r="D116" s="9"/>
-      <c r="E116" s="9"/>
-      <c r="F116" s="9"/>
-      <c r="G116" s="10"/>
-    </row>
-    <row r="117" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C117" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D117" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F117" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G117" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D118" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F118" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G118" s="4"/>
-    </row>
-    <row r="119" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B119" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C119" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="4"/>
-    </row>
-    <row r="121" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B122" s="9"/>
-      <c r="C122" s="9"/>
-      <c r="D122" s="9"/>
-      <c r="E122" s="9"/>
-      <c r="F122" s="9"/>
-      <c r="G122" s="10"/>
-    </row>
-    <row r="123" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F123" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G123" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D124" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E124" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F124" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G124" s="4"/>
-    </row>
-    <row r="125" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C125" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D125" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E125" s="4"/>
-      <c r="F125" s="4"/>
-      <c r="G125" s="4"/>
-    </row>
-    <row r="126" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C126" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D126" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
-      <c r="G126" s="4"/>
-    </row>
-    <row r="127" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="128" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B128" s="9"/>
-      <c r="C128" s="9"/>
-      <c r="D128" s="9"/>
-      <c r="E128" s="9"/>
-      <c r="F128" s="9"/>
-      <c r="G128" s="10"/>
-    </row>
-    <row r="129" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E129" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F129" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G129" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D130" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E130" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F130" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G130" s="4"/>
-    </row>
-    <row r="131" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B131" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C131" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D131" s="11"/>
-      <c r="E131" s="4"/>
-      <c r="F131" s="4"/>
-      <c r="G131" s="4"/>
-    </row>
-    <row r="132" spans="1:7" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B132" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C132" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D132" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B133" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C133" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D133" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E133" s="4"/>
-      <c r="F133" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G133" s="4"/>
-    </row>
-    <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B134" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D134" s="11"/>
-      <c r="E134" s="4"/>
-      <c r="F134" s="4"/>
-      <c r="G134" s="4"/>
-    </row>
-    <row r="135" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B135" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C135" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D135" s="11"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-    </row>
-    <row r="136" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D136" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E136" s="4"/>
-      <c r="F136" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G136" s="4"/>
+      <c r="G133" s="8" t="s">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A104:G104"/>
-    <mergeCell ref="A108:G108"/>
-    <mergeCell ref="A116:G116"/>
-    <mergeCell ref="A122:G122"/>
-    <mergeCell ref="A128:G128"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A88:G88"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A86:G86"/>
+    <mergeCell ref="A102:G102"/>
+    <mergeCell ref="A106:G106"/>
+    <mergeCell ref="A113:G113"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="A125:G125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>